<commit_message>
Start of rs485 communication interface development.
</commit_message>
<xml_diff>
--- a/v1.2/Hardware/BOM v1.2.xlsx
+++ b/v1.2/Hardware/BOM v1.2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="309">
   <si>
     <t xml:space="preserve">Component</t>
   </si>
@@ -940,19 +940,10 @@
     <t xml:space="preserve">Transformer</t>
   </si>
   <si>
-    <t xml:space="preserve">?</t>
-  </si>
-  <si>
     <t xml:space="preserve">M4</t>
   </si>
   <si>
     <t xml:space="preserve">Air cored inductor 920uH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inductor 4.47mH</t>
   </si>
   <si>
     <t xml:space="preserve">Total cost(+KDV)</t>
@@ -967,7 +958,7 @@
     <numFmt numFmtId="165" formatCode="[$TL-626]#,##0.00;[RED]\-[$TL-626]#,##0.00"/>
     <numFmt numFmtId="166" formatCode="[$₺-41F]#,##0.00;[RED]\-[$₺-41F]#,##0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -995,6 +986,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1039,7 +1036,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1057,6 +1054,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1079,15 +1080,15 @@
   </sheetPr>
   <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D88" activeCellId="0" sqref="D88"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B65" activeCellId="0" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="39.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.19"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="11.52"/>
@@ -3107,50 +3108,58 @@
       <c r="B85" s="0" t="s">
         <v>305</v>
       </c>
-      <c r="D85" s="0" t="s">
-        <v>306</v>
-      </c>
-      <c r="E85" s="3"/>
-      <c r="G85" s="0"/>
+      <c r="D85" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="E85" s="3" t="n">
+        <v>240</v>
+      </c>
+      <c r="F85" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G85" s="1" t="n">
+        <f aca="false">E85*F85</f>
+        <v>240</v>
+      </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="B86" s="0" t="s">
         <v>307</v>
       </c>
-      <c r="B86" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="D86" s="0" t="s">
-        <v>306</v>
-      </c>
-      <c r="E86" s="3"/>
-      <c r="G86" s="0"/>
+      <c r="D86" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="E86" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="F86" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G86" s="1" t="n">
+        <f aca="false">E86*F86</f>
+        <v>40</v>
+      </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="s">
-        <v>309</v>
-      </c>
-      <c r="B87" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="D87" s="0" t="s">
-        <v>306</v>
-      </c>
       <c r="E87" s="3"/>
-      <c r="G87" s="0"/>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="0" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C89" s="1" t="n">
         <f aca="false">1.18 * SUM(G:G)</f>
-        <v>921.0252042</v>
+        <v>1251.4252042</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D84" r:id="rId1" display="www.artek.com"/>
+    <hyperlink ref="D85" r:id="rId2" display="www.artek.com"/>
+    <hyperlink ref="D86" r:id="rId3" display="www.artek.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>